<commit_message>
Small changes in excel document
</commit_message>
<xml_diff>
--- a/171221-klassER.xlsx
+++ b/171221-klassER.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna-Maja Lithner\Desktop\skola\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna-Maja Lithner\Desktop\skola\Databasteknik\Laborationer, övningar\DBTEK171221_exc_klass\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ELEV</t>
   </si>
@@ -39,12 +39,6 @@
   </si>
   <si>
     <t>LÄRARE</t>
-  </si>
-  <si>
-    <t>Kalle</t>
-  </si>
-  <si>
-    <t>710429-0023</t>
   </si>
   <si>
     <t>Kursnamn</t>
@@ -129,7 +123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -171,21 +165,53 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -200,25 +226,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -230,66 +241,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -378,19 +333,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -444,37 +386,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,241 +691,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K30"/>
+  <dimension ref="A3:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="50" zoomScaleNormal="90" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="11" width="15.6328125" customWidth="1"/>
+    <col min="1" max="10" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B4" s="8" t="s">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
+      <c r="B4" s="8"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="10"/>
-      <c r="K4" s="25" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="12"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="13"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="11" t="s">
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="21" t="s">
+      <c r="C18" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="16"/>
-      <c r="K6" s="27"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="15"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="16"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="16"/>
-      <c r="K7" s="27"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B8" s="15"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="16"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="16"/>
-      <c r="K8" s="27"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B9" s="15"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="16"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="16"/>
-      <c r="K9" s="27"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B10" s="15"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="16"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="16"/>
-      <c r="K10" s="27"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B11" s="15"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="16"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="16"/>
-      <c r="K11" s="27"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B12" s="15"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="16"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="16"/>
-      <c r="K12" s="27"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B13" s="15"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="16"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="16"/>
-      <c r="K13" s="27"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B14" s="15"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="16"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="16"/>
-      <c r="K14" s="27"/>
-    </row>
-    <row r="15" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="19"/>
-      <c r="K15" s="28"/>
-    </row>
-    <row r="21" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="10"/>
-      <c r="J22" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B24" s="15"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="16"/>
-      <c r="J24" s="27"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B25" s="15"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="16"/>
-      <c r="J25" s="27"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B26" s="15"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="16"/>
-      <c r="J26" s="27"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B27" s="15"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="16"/>
-      <c r="J27" s="27"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B28" s="15"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="16"/>
-      <c r="J28" s="27"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B29" s="15"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="16"/>
-      <c r="J29" s="27"/>
-    </row>
-    <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
-      <c r="J30" s="28"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="22"/>
+      <c r="C19" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C171221 - klassER
+Tabeller baserade på diagram övver klasser
+171221-lab-klassER</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>